<commit_message>
SIAM v3 (last release on 20180124)
</commit_message>
<xml_diff>
--- a/SIAM/_SIAM_pop.xlsx
+++ b/SIAM/_SIAM_pop.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>Organization</t>
   </si>
@@ -133,15 +133,24 @@
     <t>rieks</t>
   </si>
   <si>
+    <t>joosten</t>
+  </si>
+  <si>
     <t>michiel</t>
   </si>
   <si>
+    <t>nolan</t>
+  </si>
+  <si>
     <t>accAllowedRoles</t>
   </si>
   <si>
     <t>ad</t>
   </si>
   <si>
+    <t>minderbrood</t>
+  </si>
+  <si>
     <t>accIsGodAccount</t>
   </si>
   <si>
@@ -151,6 +160,18 @@
     <t>accOrg</t>
   </si>
   <si>
+    <t>Jorrit</t>
+  </si>
+  <si>
+    <t>de Boer</t>
+  </si>
+  <si>
+    <t>deboer</t>
+  </si>
+  <si>
+    <t>jorrit</t>
+  </si>
+  <si>
     <t>User, Administrator</t>
   </si>
   <si>
@@ -172,9 +193,6 @@
     <t>UID</t>
   </si>
   <si>
-    <t>uidIdP</t>
-  </si>
-  <si>
     <t>uidUserid</t>
   </si>
   <si>
@@ -220,13 +238,7 @@
     <t>rj@g</t>
   </si>
   <si>
-    <t>Jelle</t>
-  </si>
-  <si>
-    <t>Nauta</t>
-  </si>
-  <si>
-    <t>jelle</t>
+    <t>uidIssuer</t>
   </si>
 </sst>
 </file>
@@ -665,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,13 +765,13 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="str">
         <f>IF($B6="","",CONCATENATE($B6," ",$C6))</f>
-        <v>Jelle Nauta</v>
+        <v>Jorrit de Boer</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -832,23 +844,23 @@
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H12" s="6" t="str">
         <f>IF((ROWS($H$14:$H$17)-COUNTBLANK($H$14:$H$17))=0,"","autoLoginAccount")</f>
         <v/>
       </c>
       <c r="I12" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -868,10 +880,10 @@
         <v>0</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="H13" s="2" t="str">
         <f>$A13</f>
@@ -887,22 +899,21 @@
         <v>Acc_ad</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="7" t="str">
-        <f>IF($B14="","","*****")</f>
-        <v>*****</v>
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="D14" s="7" t="str">
         <f>$A3</f>
         <v>Ad Minderbrood</v>
       </c>
       <c r="E14" s="7" t="str">
-        <f>IF($B14="","",$A$10)</f>
+        <f>$A$10</f>
         <v>TNO</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H14" s="7"/>
     </row>
@@ -914,23 +925,22 @@
       <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="7" t="str">
-        <f t="shared" ref="C15:C18" si="2">IF($B15="","","*****")</f>
-        <v>*****</v>
+      <c r="C15" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D15" s="7" t="str">
-        <f t="shared" ref="D15" si="3">$A4</f>
+        <f t="shared" ref="D15" si="2">$A4</f>
         <v>Rieks Joosten</v>
       </c>
       <c r="E15" s="7" t="str">
-        <f t="shared" ref="E15:E18" si="4">IF($B15="","",$A$10)</f>
+        <f t="shared" ref="E15:E18" si="3">$A$10</f>
         <v>TNO</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" t="str">
@@ -944,46 +954,44 @@
         <v>Acc_michiel</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>*****</v>
+        <v>29</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D16" s="7" t="str">
-        <f t="shared" ref="D16" si="5">$A5</f>
+        <f t="shared" ref="D16" si="4">$A5</f>
         <v>Michiel Stornebrink</v>
       </c>
       <c r="E16" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>TNO</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>Acc_jelle</v>
+        <v>Acc_jorrit</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>*****</v>
+        <v>40</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="D17" s="7" t="str">
         <f>$A6</f>
-        <v>Jelle Nauta</v>
+        <v>Jorrit de Boer</v>
       </c>
       <c r="E17" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>TNO</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -996,45 +1004,25 @@
         <f>IF($B18="","",CONCATENATE("Acc_",$B18))</f>
         <v/>
       </c>
-      <c r="C18" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
       <c r="D18" s="7" t="str">
         <f>$A7</f>
         <v/>
       </c>
       <c r="E18" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+        <f t="shared" si="3"/>
+        <v>TNO</v>
       </c>
       <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
@@ -1042,69 +1030,85 @@
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>43</v>
-      </c>
+    <row r="21" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>43</v>
+      <c r="C26" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1"/>
+    <hyperlink ref="A22" r:id="rId1"/>
     <hyperlink ref="F16" r:id="rId2" display="ms@google"/>
-    <hyperlink ref="A22" r:id="rId3"/>
-    <hyperlink ref="A23" r:id="rId4"/>
-    <hyperlink ref="A24" r:id="rId5"/>
-    <hyperlink ref="A25" r:id="rId6"/>
+    <hyperlink ref="A23" r:id="rId3"/>
+    <hyperlink ref="A24" r:id="rId4"/>
+    <hyperlink ref="A25" r:id="rId5"/>
+    <hyperlink ref="A26" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>

</xml_diff>